<commit_message>
Commit before psuhing for ID recognition of chatgpt
</commit_message>
<xml_diff>
--- a/data/input/source_data.xlsx
+++ b/data/input/source_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="84">
   <si>
     <t>Designation article</t>
   </si>
@@ -263,6 +263,9 @@
   </si>
   <si>
     <t>Bose QuietComfort 45 (ANC, 22 h, Filaire, Sans fil)</t>
+  </si>
+  <si>
+    <t>Laboratory, measurement, observation and testing equipment</t>
   </si>
 </sst>
 </file>
@@ -287,13 +290,13 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -362,45 +365,42 @@
     <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
+      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -408,7 +408,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general" wrapText="1"/>
@@ -715,23 +718,23 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:K50"/>
+  <dimension ref="A1:K51"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="18" width="181.29071428571427" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="19" width="8.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="18" width="71.14785714285713" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="20" width="37.005" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="21" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="22" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="18" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="18" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="18" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="18" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="18" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="17" width="181.29071428571427" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="18" width="8.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="17" width="71.14785714285713" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="19" width="37.005" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="20" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="21" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="22" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="17" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="22" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="17" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="17" width="14.147857142857141" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="33.75" customFormat="1" s="1">
@@ -753,23 +756,23 @@
       <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5" customFormat="1" s="1">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="8">
+      <c r="B2" s="6">
         <v>381</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="4">
@@ -778,23 +781,23 @@
       <c r="F2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="33" customFormat="1" s="1">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3" s="6">
         <v>1700</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E3" s="4">
@@ -803,23 +806,23 @@
       <c r="F3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5" customFormat="1" s="1">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="6">
         <v>65</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E4" s="4">
@@ -828,23 +831,23 @@
       <c r="F4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5" customFormat="1" s="1">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B5" s="7">
         <v>34</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E5" s="4">
@@ -853,1134 +856,1157 @@
       <c r="F5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="11">
+      <c r="B6" s="9">
         <v>65.6</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="13">
+      <c r="E6" s="11">
         <v>44932</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="11">
+      <c r="B7" s="9">
         <v>5000</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E7" s="11">
         <v>44933</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="14">
+      <c r="B8" s="13">
         <v>100</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="13">
+      <c r="E8" s="11">
         <v>44934</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="14">
+      <c r="B9" s="13">
         <v>16</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="13">
+      <c r="E9" s="11">
         <v>44935</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="14">
+      <c r="B10" s="13">
         <v>5</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="13">
+      <c r="E10" s="11">
         <v>44936</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="10"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="14">
+      <c r="B11" s="13">
         <v>10</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D11" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="E11" s="13">
+      <c r="E11" s="11">
         <v>44937</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="10"/>
-      <c r="K11" s="10"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="14">
+      <c r="B12" s="13">
         <v>47</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C12" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="12" t="s">
+      <c r="D12" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="13">
+      <c r="E12" s="11">
         <v>44938</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="10"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
-      <c r="A13" s="10" t="s">
+      <c r="A13" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="14">
+      <c r="B13" s="13">
         <v>19000</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="12" t="s">
+      <c r="D13" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="E13" s="13">
+      <c r="E13" s="11">
         <v>44939</v>
       </c>
       <c r="F13" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="10"/>
-      <c r="K13" s="10"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="14">
+      <c r="B14" s="13">
         <v>2000</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C14" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="12" t="s">
+      <c r="D14" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="E14" s="13">
+      <c r="E14" s="11">
         <v>44940</v>
       </c>
       <c r="F14" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="10"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
-      <c r="A15" s="10" t="s">
+      <c r="A15" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="14">
+      <c r="B15" s="13">
         <v>100</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="C15" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D15" s="12" t="s">
+      <c r="D15" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="E15" s="13">
+      <c r="E15" s="11">
         <v>44941</v>
       </c>
       <c r="F15" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="10"/>
-      <c r="K15" s="10"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
-      <c r="A16" s="10" t="s">
+      <c r="A16" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="14">
+      <c r="B16" s="13">
         <v>50</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="C16" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D16" s="12" t="s">
+      <c r="D16" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="E16" s="13">
+      <c r="E16" s="11">
         <v>44942</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G16" s="10"/>
-      <c r="H16" s="10"/>
-      <c r="I16" s="10"/>
-      <c r="J16" s="10"/>
-      <c r="K16" s="10"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="14">
+      <c r="B17" s="13">
         <v>100</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="C17" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D17" s="12" t="s">
+      <c r="D17" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="E17" s="13">
+      <c r="E17" s="11">
         <v>44943</v>
       </c>
       <c r="F17" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G17" s="10"/>
-      <c r="H17" s="10"/>
-      <c r="I17" s="10"/>
-      <c r="J17" s="10"/>
-      <c r="K17" s="10"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
-      <c r="A18" s="10" t="s">
+      <c r="A18" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="14">
+      <c r="B18" s="13">
         <v>300</v>
       </c>
-      <c r="C18" s="10" t="s">
+      <c r="C18" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="D18" s="12" t="s">
+      <c r="D18" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="E18" s="13">
+      <c r="E18" s="11">
         <v>44944</v>
       </c>
       <c r="F18" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G18" s="10"/>
-      <c r="H18" s="10"/>
-      <c r="I18" s="10"/>
-      <c r="J18" s="10"/>
-      <c r="K18" s="10"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B19" s="11">
+      <c r="B19" s="9">
         <v>0.31</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C19" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D19" s="12" t="s">
+      <c r="D19" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="E19" s="13">
+      <c r="E19" s="11">
         <v>44945</v>
       </c>
       <c r="F19" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G19" s="10"/>
-      <c r="H19" s="10"/>
-      <c r="I19" s="10"/>
-      <c r="J19" s="10"/>
-      <c r="K19" s="10"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="8"/>
+      <c r="K19" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
-      <c r="A20" s="7" t="s">
+      <c r="A20" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B20" s="11">
+      <c r="B20" s="9">
         <v>0.48</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C20" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D20" s="12" t="s">
+      <c r="D20" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="E20" s="13">
+      <c r="E20" s="11">
         <v>44946</v>
       </c>
       <c r="F20" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G20" s="10"/>
-      <c r="H20" s="10"/>
-      <c r="I20" s="10"/>
-      <c r="J20" s="10"/>
-      <c r="K20" s="10"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="8"/>
+      <c r="K20" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
-      <c r="A21" s="7" t="s">
+      <c r="A21" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B21" s="11">
+      <c r="B21" s="9">
         <v>0.71</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="C21" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D21" s="12" t="s">
+      <c r="D21" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="E21" s="13">
+      <c r="E21" s="11">
         <v>44947</v>
       </c>
       <c r="F21" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G21" s="10"/>
-      <c r="H21" s="10"/>
-      <c r="I21" s="10"/>
-      <c r="J21" s="10"/>
-      <c r="K21" s="10"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="8"/>
+      <c r="K21" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
-      <c r="A22" s="7" t="s">
+      <c r="A22" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B22" s="14">
+      <c r="B22" s="13">
         <v>150</v>
       </c>
-      <c r="C22" s="10" t="s">
+      <c r="C22" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D22" s="12" t="s">
+      <c r="D22" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="E22" s="13">
+      <c r="E22" s="11">
         <v>44948</v>
       </c>
       <c r="F22" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G22" s="10"/>
-      <c r="H22" s="10"/>
-      <c r="I22" s="10"/>
-      <c r="J22" s="10"/>
-      <c r="K22" s="10"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="12"/>
+      <c r="J22" s="8"/>
+      <c r="K22" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
-      <c r="A23" s="10" t="s">
+      <c r="A23" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="B23" s="14">
+      <c r="B23" s="13">
         <v>2000</v>
       </c>
-      <c r="C23" s="10" t="s">
+      <c r="C23" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="D23" s="12" t="s">
+      <c r="D23" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="E23" s="13">
+      <c r="E23" s="11">
         <v>44949</v>
       </c>
       <c r="F23" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G23" s="10"/>
-      <c r="H23" s="10"/>
-      <c r="I23" s="10"/>
-      <c r="J23" s="10"/>
-      <c r="K23" s="10"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="12"/>
+      <c r="J23" s="8"/>
+      <c r="K23" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
-      <c r="A24" s="10" t="s">
+      <c r="A24" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="B24" s="14">
+      <c r="B24" s="13">
         <v>100</v>
       </c>
-      <c r="C24" s="10" t="s">
+      <c r="C24" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D24" s="12" t="s">
+      <c r="D24" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="E24" s="13">
+      <c r="E24" s="11">
         <v>44950</v>
       </c>
       <c r="F24" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G24" s="10"/>
-      <c r="H24" s="10"/>
-      <c r="I24" s="10"/>
-      <c r="J24" s="10"/>
-      <c r="K24" s="10"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="8"/>
+      <c r="I24" s="12"/>
+      <c r="J24" s="8"/>
+      <c r="K24" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
-      <c r="A25" s="10" t="s">
+      <c r="A25" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="B25" s="14">
+      <c r="B25" s="13">
         <v>69</v>
       </c>
-      <c r="C25" s="10" t="s">
+      <c r="C25" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D25" s="12" t="s">
+      <c r="D25" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="E25" s="13">
+      <c r="E25" s="11">
         <v>44951</v>
       </c>
       <c r="F25" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G25" s="10"/>
-      <c r="H25" s="10"/>
-      <c r="I25" s="10"/>
-      <c r="J25" s="10"/>
-      <c r="K25" s="10"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="8"/>
+      <c r="I25" s="12"/>
+      <c r="J25" s="8"/>
+      <c r="K25" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
-      <c r="A26" s="10" t="s">
+      <c r="A26" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="B26" s="14">
+      <c r="B26" s="13">
         <v>400</v>
       </c>
-      <c r="C26" s="10" t="s">
+      <c r="C26" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D26" s="12" t="s">
+      <c r="D26" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="E26" s="13">
+      <c r="E26" s="11">
         <v>44952</v>
       </c>
       <c r="F26" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G26" s="10"/>
-      <c r="H26" s="10"/>
-      <c r="I26" s="10"/>
-      <c r="J26" s="10"/>
-      <c r="K26" s="10"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="8"/>
+      <c r="I26" s="12"/>
+      <c r="J26" s="8"/>
+      <c r="K26" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
-      <c r="A27" s="10" t="s">
+      <c r="A27" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B27" s="14">
+      <c r="B27" s="13">
         <v>3000</v>
       </c>
-      <c r="C27" s="10" t="s">
+      <c r="C27" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="D27" s="12" t="s">
+      <c r="D27" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="E27" s="13">
+      <c r="E27" s="11">
         <v>44953</v>
       </c>
       <c r="F27" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G27" s="10"/>
-      <c r="H27" s="10"/>
-      <c r="I27" s="10"/>
-      <c r="J27" s="10"/>
-      <c r="K27" s="10"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="8"/>
+      <c r="I27" s="12"/>
+      <c r="J27" s="8"/>
+      <c r="K27" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5">
-      <c r="A28" s="10" t="s">
+      <c r="A28" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="B28" s="14">
+      <c r="B28" s="13">
         <v>1000</v>
       </c>
-      <c r="C28" s="10" t="s">
+      <c r="C28" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="D28" s="12" t="s">
+      <c r="D28" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="E28" s="13">
+      <c r="E28" s="11">
         <v>44954</v>
       </c>
       <c r="F28" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G28" s="10"/>
-      <c r="H28" s="10"/>
-      <c r="I28" s="10"/>
-      <c r="J28" s="10"/>
-      <c r="K28" s="10"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="8"/>
+      <c r="I28" s="12"/>
+      <c r="J28" s="8"/>
+      <c r="K28" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="19.5">
-      <c r="A29" s="10" t="s">
+      <c r="A29" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="B29" s="14">
+      <c r="B29" s="13">
         <v>200</v>
       </c>
-      <c r="C29" s="10" t="s">
+      <c r="C29" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="D29" s="12" t="s">
+      <c r="D29" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="E29" s="13">
+      <c r="E29" s="11">
         <v>44955</v>
       </c>
       <c r="F29" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G29" s="10"/>
-      <c r="H29" s="10"/>
-      <c r="I29" s="10"/>
-      <c r="J29" s="10"/>
-      <c r="K29" s="10"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="8"/>
+      <c r="I29" s="12"/>
+      <c r="J29" s="8"/>
+      <c r="K29" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="19.5">
-      <c r="A30" s="10" t="s">
+      <c r="A30" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="B30" s="14">
+      <c r="B30" s="13">
         <v>170</v>
       </c>
-      <c r="C30" s="10" t="s">
+      <c r="C30" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D30" s="12" t="s">
+      <c r="D30" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="E30" s="13">
+      <c r="E30" s="11">
         <v>44956</v>
       </c>
       <c r="F30" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G30" s="10"/>
-      <c r="H30" s="10"/>
-      <c r="I30" s="10"/>
-      <c r="J30" s="10"/>
-      <c r="K30" s="10"/>
+      <c r="G30" s="12"/>
+      <c r="H30" s="8"/>
+      <c r="I30" s="12"/>
+      <c r="J30" s="8"/>
+      <c r="K30" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="19.5">
-      <c r="A31" s="10" t="s">
+      <c r="A31" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="B31" s="14">
+      <c r="B31" s="13">
         <v>60</v>
       </c>
-      <c r="C31" s="10" t="s">
+      <c r="C31" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D31" s="12" t="s">
+      <c r="D31" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="E31" s="13">
+      <c r="E31" s="11">
         <v>44957</v>
       </c>
       <c r="F31" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G31" s="10"/>
-      <c r="H31" s="10"/>
-      <c r="I31" s="10"/>
-      <c r="J31" s="10"/>
-      <c r="K31" s="10"/>
+      <c r="G31" s="12"/>
+      <c r="H31" s="8"/>
+      <c r="I31" s="12"/>
+      <c r="J31" s="8"/>
+      <c r="K31" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="19.5">
-      <c r="A32" s="10" t="s">
+      <c r="A32" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="B32" s="14">
+      <c r="B32" s="13">
         <v>46</v>
       </c>
-      <c r="C32" s="10" t="s">
+      <c r="C32" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D32" s="12" t="s">
+      <c r="D32" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="E32" s="13">
+      <c r="E32" s="11">
         <v>44958</v>
       </c>
       <c r="F32" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G32" s="10"/>
-      <c r="H32" s="10"/>
-      <c r="I32" s="10"/>
-      <c r="J32" s="10"/>
-      <c r="K32" s="10"/>
+      <c r="G32" s="12"/>
+      <c r="H32" s="8"/>
+      <c r="I32" s="12"/>
+      <c r="J32" s="8"/>
+      <c r="K32" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="19.5">
-      <c r="A33" s="10" t="s">
+      <c r="A33" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="B33" s="14">
+      <c r="B33" s="13">
         <v>26</v>
       </c>
-      <c r="C33" s="10" t="s">
+      <c r="C33" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="D33" s="12" t="s">
+      <c r="D33" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="E33" s="13">
+      <c r="E33" s="11">
         <v>44959</v>
       </c>
       <c r="F33" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G33" s="10"/>
-      <c r="H33" s="10"/>
-      <c r="I33" s="10"/>
-      <c r="J33" s="10"/>
-      <c r="K33" s="10"/>
+      <c r="G33" s="12"/>
+      <c r="H33" s="8"/>
+      <c r="I33" s="12"/>
+      <c r="J33" s="8"/>
+      <c r="K33" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="19.5">
-      <c r="A34" s="10" t="s">
+      <c r="A34" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="B34" s="14">
+      <c r="B34" s="13">
         <v>1</v>
       </c>
-      <c r="C34" s="10" t="s">
+      <c r="C34" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="D34" s="12" t="s">
+      <c r="D34" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="E34" s="13">
+      <c r="E34" s="11">
         <v>44960</v>
       </c>
       <c r="F34" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G34" s="10"/>
-      <c r="H34" s="10"/>
-      <c r="I34" s="10"/>
-      <c r="J34" s="10"/>
-      <c r="K34" s="10"/>
+      <c r="G34" s="12"/>
+      <c r="H34" s="8"/>
+      <c r="I34" s="12"/>
+      <c r="J34" s="8"/>
+      <c r="K34" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="19.5">
-      <c r="A35" s="10" t="s">
+      <c r="A35" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="B35" s="11">
+      <c r="B35" s="9">
         <v>16.5</v>
       </c>
-      <c r="C35" s="10" t="s">
+      <c r="C35" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D35" s="12" t="s">
+      <c r="D35" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="E35" s="13">
+      <c r="E35" s="11">
         <v>44961</v>
       </c>
       <c r="F35" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G35" s="10"/>
-      <c r="H35" s="15"/>
-      <c r="I35" s="10"/>
-      <c r="J35" s="10"/>
-      <c r="K35" s="10"/>
+      <c r="G35" s="12"/>
+      <c r="H35" s="10"/>
+      <c r="I35" s="12"/>
+      <c r="J35" s="8"/>
+      <c r="K35" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="19.5">
-      <c r="A36" s="10" t="s">
+      <c r="A36" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="B36" s="11">
+      <c r="B36" s="9">
         <v>7.15</v>
       </c>
-      <c r="C36" s="10" t="s">
+      <c r="C36" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="D36" s="12" t="s">
+      <c r="D36" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="E36" s="13">
+      <c r="E36" s="11">
         <v>44962</v>
       </c>
       <c r="F36" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G36" s="10"/>
-      <c r="H36" s="15"/>
-      <c r="I36" s="10"/>
-      <c r="J36" s="10"/>
-      <c r="K36" s="10"/>
+      <c r="G36" s="12"/>
+      <c r="H36" s="10"/>
+      <c r="I36" s="12"/>
+      <c r="J36" s="8"/>
+      <c r="K36" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="19.5">
-      <c r="A37" s="10" t="s">
+      <c r="A37" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="B37" s="11">
+      <c r="B37" s="9">
         <v>140.53</v>
       </c>
-      <c r="C37" s="10" t="s">
+      <c r="C37" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="D37" s="12" t="s">
+      <c r="D37" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="E37" s="13">
+      <c r="E37" s="11">
         <v>44963</v>
       </c>
       <c r="F37" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G37" s="10"/>
-      <c r="H37" s="15"/>
-      <c r="I37" s="10"/>
-      <c r="J37" s="10"/>
-      <c r="K37" s="10"/>
+      <c r="G37" s="12"/>
+      <c r="H37" s="10"/>
+      <c r="I37" s="12"/>
+      <c r="J37" s="8"/>
+      <c r="K37" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="19.5">
-      <c r="A38" s="10" t="s">
+      <c r="A38" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="B38" s="11">
+      <c r="B38" s="9">
         <v>84.78</v>
       </c>
-      <c r="C38" s="10" t="s">
+      <c r="C38" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D38" s="12" t="s">
+      <c r="D38" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="E38" s="13">
+      <c r="E38" s="11">
         <v>44964</v>
       </c>
       <c r="F38" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G38" s="10"/>
-      <c r="H38" s="15"/>
-      <c r="I38" s="10"/>
-      <c r="J38" s="10"/>
-      <c r="K38" s="10"/>
+      <c r="G38" s="12"/>
+      <c r="H38" s="10"/>
+      <c r="I38" s="12"/>
+      <c r="J38" s="8"/>
+      <c r="K38" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="19.5">
-      <c r="A39" s="10" t="s">
+      <c r="A39" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="B39" s="11">
+      <c r="B39" s="9">
         <v>156.57</v>
       </c>
-      <c r="C39" s="10" t="s">
+      <c r="C39" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D39" s="12" t="s">
+      <c r="D39" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="E39" s="13">
+      <c r="E39" s="11">
         <v>44965</v>
       </c>
       <c r="F39" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G39" s="10"/>
-      <c r="H39" s="15"/>
-      <c r="I39" s="10"/>
-      <c r="J39" s="10"/>
-      <c r="K39" s="10"/>
+      <c r="G39" s="12"/>
+      <c r="H39" s="10"/>
+      <c r="I39" s="12"/>
+      <c r="J39" s="8"/>
+      <c r="K39" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="19.5">
-      <c r="A40" s="10" t="s">
+      <c r="A40" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="B40" s="11">
+      <c r="B40" s="9">
         <v>0.7</v>
       </c>
-      <c r="C40" s="10" t="s">
+      <c r="C40" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D40" s="12" t="s">
+      <c r="D40" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="E40" s="13">
+      <c r="E40" s="11">
         <v>44966</v>
       </c>
       <c r="F40" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G40" s="10"/>
-      <c r="H40" s="15"/>
-      <c r="I40" s="10"/>
-      <c r="J40" s="10"/>
-      <c r="K40" s="10"/>
+      <c r="G40" s="12"/>
+      <c r="H40" s="10"/>
+      <c r="I40" s="12"/>
+      <c r="J40" s="8"/>
+      <c r="K40" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="19.5">
-      <c r="A41" s="10" t="s">
+      <c r="A41" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="B41" s="11">
+      <c r="B41" s="9">
         <v>21.81</v>
       </c>
-      <c r="C41" s="10" t="s">
+      <c r="C41" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="D41" s="12" t="s">
+      <c r="D41" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="E41" s="13">
+      <c r="E41" s="11">
         <v>44967</v>
       </c>
       <c r="F41" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G41" s="10"/>
-      <c r="H41" s="15"/>
-      <c r="I41" s="10"/>
-      <c r="J41" s="15"/>
-      <c r="K41" s="15"/>
+      <c r="G41" s="12"/>
+      <c r="H41" s="10"/>
+      <c r="I41" s="12"/>
+      <c r="J41" s="10"/>
+      <c r="K41" s="10"/>
     </row>
     <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="19.5">
-      <c r="A42" s="10" t="s">
+      <c r="A42" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="B42" s="14">
+      <c r="B42" s="13">
         <v>475</v>
       </c>
-      <c r="C42" s="10" t="s">
+      <c r="C42" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D42" s="12" t="s">
+      <c r="D42" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="E42" s="13">
+      <c r="E42" s="11">
         <v>44968</v>
       </c>
       <c r="F42" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G42" s="10"/>
-      <c r="H42" s="15"/>
-      <c r="I42" s="10"/>
-      <c r="J42" s="15"/>
-      <c r="K42" s="15"/>
+      <c r="G42" s="12"/>
+      <c r="H42" s="10"/>
+      <c r="I42" s="12"/>
+      <c r="J42" s="10"/>
+      <c r="K42" s="10"/>
     </row>
     <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="19.5">
-      <c r="A43" s="10" t="s">
+      <c r="A43" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="B43" s="11">
+      <c r="B43" s="9">
         <v>12.67</v>
       </c>
-      <c r="C43" s="10" t="s">
+      <c r="C43" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D43" s="12" t="s">
+      <c r="D43" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="E43" s="13">
+      <c r="E43" s="11">
         <v>44969</v>
       </c>
       <c r="F43" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G43" s="10"/>
-      <c r="H43" s="15"/>
-      <c r="I43" s="10"/>
-      <c r="J43" s="15"/>
-      <c r="K43" s="15"/>
+      <c r="G43" s="12"/>
+      <c r="H43" s="10"/>
+      <c r="I43" s="12"/>
+      <c r="J43" s="10"/>
+      <c r="K43" s="10"/>
     </row>
     <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="19.5">
-      <c r="A44" s="16" t="s">
+      <c r="A44" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="B44" s="17">
+      <c r="B44" s="15">
         <v>186.43</v>
       </c>
-      <c r="C44" s="16" t="s">
+      <c r="C44" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="D44" s="16" t="s">
+      <c r="D44" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="E44" s="13">
+      <c r="E44" s="11">
         <v>44970</v>
       </c>
       <c r="F44" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G44" s="10"/>
-      <c r="H44" s="15"/>
-      <c r="I44" s="10"/>
-      <c r="J44" s="15"/>
-      <c r="K44" s="15"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="19.5">
-      <c r="A45" s="15" t="s">
+      <c r="G44" s="12"/>
+      <c r="H44" s="10"/>
+      <c r="I44" s="12"/>
+      <c r="J44" s="10"/>
+      <c r="K44" s="10"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="20.25">
+      <c r="A45" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="B45" s="11">
+      <c r="B45" s="9">
         <v>28201.68</v>
       </c>
-      <c r="C45" s="15" t="s">
+      <c r="C45" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D45" s="15" t="s">
+      <c r="D45" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="E45" s="13">
+      <c r="E45" s="11">
         <v>44971</v>
       </c>
       <c r="F45" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G45" s="10"/>
-      <c r="H45" s="15"/>
-      <c r="I45" s="10"/>
-      <c r="J45" s="15"/>
-      <c r="K45" s="15"/>
+      <c r="G45" s="12"/>
+      <c r="H45" s="10"/>
+      <c r="I45" s="12"/>
+      <c r="J45" s="10"/>
+      <c r="K45" s="10"/>
     </row>
     <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="19.5">
-      <c r="A46" s="15" t="s">
+      <c r="A46" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="B46" s="14">
+      <c r="B46" s="13">
         <v>984</v>
       </c>
-      <c r="C46" s="15" t="s">
+      <c r="C46" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="D46" s="15" t="s">
+      <c r="D46" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="E46" s="13">
+      <c r="E46" s="11">
         <v>44972</v>
       </c>
       <c r="F46" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G46" s="10"/>
-      <c r="H46" s="15"/>
-      <c r="I46" s="10"/>
-      <c r="J46" s="15"/>
-      <c r="K46" s="15"/>
+      <c r="G46" s="12"/>
+      <c r="H46" s="10"/>
+      <c r="I46" s="12"/>
+      <c r="J46" s="10"/>
+      <c r="K46" s="10"/>
     </row>
     <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="19.5">
-      <c r="A47" s="15" t="s">
+      <c r="A47" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="B47" s="11">
+      <c r="B47" s="9">
         <v>25.04</v>
       </c>
-      <c r="C47" s="15" t="s">
+      <c r="C47" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="D47" s="15" t="s">
+      <c r="D47" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="E47" s="13">
+      <c r="E47" s="11">
         <v>44973</v>
       </c>
       <c r="F47" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G47" s="10"/>
-      <c r="H47" s="15"/>
-      <c r="I47" s="10"/>
-      <c r="J47" s="15"/>
-      <c r="K47" s="15"/>
+      <c r="G47" s="12"/>
+      <c r="H47" s="10"/>
+      <c r="I47" s="12"/>
+      <c r="J47" s="10"/>
+      <c r="K47" s="10"/>
     </row>
     <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="19.5">
-      <c r="A48" s="15" t="s">
+      <c r="A48" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="B48" s="11">
+      <c r="B48" s="9">
         <v>463.32</v>
       </c>
-      <c r="C48" s="15" t="s">
+      <c r="C48" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="D48" s="15" t="s">
+      <c r="D48" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="E48" s="13">
+      <c r="E48" s="11">
         <v>44974</v>
       </c>
       <c r="F48" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G48" s="10"/>
-      <c r="H48" s="15"/>
-      <c r="I48" s="10"/>
-      <c r="J48" s="10"/>
-      <c r="K48" s="10"/>
+      <c r="G48" s="12"/>
+      <c r="H48" s="10"/>
+      <c r="I48" s="12"/>
+      <c r="J48" s="8"/>
+      <c r="K48" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="19.5">
-      <c r="A49" s="15" t="s">
+      <c r="A49" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="B49" s="11">
+      <c r="B49" s="9">
         <v>183.55</v>
       </c>
-      <c r="C49" s="15" t="s">
+      <c r="C49" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="D49" s="15" t="s">
+      <c r="D49" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="E49" s="13">
+      <c r="E49" s="11">
         <v>44975</v>
       </c>
       <c r="F49" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G49" s="10"/>
-      <c r="H49" s="15"/>
-      <c r="I49" s="10"/>
-      <c r="J49" s="10"/>
-      <c r="K49" s="10"/>
+      <c r="G49" s="12"/>
+      <c r="H49" s="10"/>
+      <c r="I49" s="12"/>
+      <c r="J49" s="8"/>
+      <c r="K49" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="19.5">
-      <c r="A50" s="10" t="s">
+      <c r="A50" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="B50" s="16">
+        <v>11000</v>
+      </c>
+      <c r="C50" s="8"/>
+      <c r="D50" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="E50" s="11">
+        <v>44975</v>
+      </c>
+      <c r="F50" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G50" s="12"/>
+      <c r="H50" s="8"/>
+      <c r="I50" s="12"/>
+      <c r="J50" s="8"/>
+      <c r="K50" s="8"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="19.5">
+      <c r="A51" s="8"/>
+      <c r="B51" s="9">
+        <v>1000</v>
+      </c>
+      <c r="C51" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B50" s="11">
-        <v>1000</v>
-      </c>
-      <c r="C50" s="10"/>
-      <c r="D50" s="15" t="s">
+      <c r="D51" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="E50" s="13">
+      <c r="E51" s="11">
         <v>44976</v>
       </c>
-      <c r="F50" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G50" s="10"/>
-      <c r="H50" s="10"/>
-      <c r="I50" s="10"/>
-      <c r="J50" s="10"/>
-      <c r="K50" s="10"/>
+      <c r="F51" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G51" s="12"/>
+      <c r="H51" s="8"/>
+      <c r="I51" s="12"/>
+      <c r="J51" s="8"/>
+      <c r="K51" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>